<commit_message>
Added installation , running , queries help and my contact info in README.MD in Web Scrapper
</commit_message>
<xml_diff>
--- a/Web Scrapper/data.xlsx
+++ b/Web Scrapper/data.xlsx
@@ -596,22 +596,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Accenture</t>
+          <t>Wipro</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Professional Attributes : a Responsible to interact with other team stakeholders and ma...</t>
+          <t xml:space="preserve"> Build the infrastructure required for optimal extraction, transformation, and loading o...</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6-8 Yrs</t>
+          <t>3-8 Yrs</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bangalore/Bengaluru</t>
+          <t>Gurgaon/Gurugram, Bangalore/Bengaluru</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -621,29 +621,29 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['HTML5', 'Pyspark', 'JavaScript', 'Django', 'object - relational mapping ORM', 'Python', 'Flask', 'Pyramid']</t>
+          <t>['Snowflake', 'AWS', 'EC2', 'RDS', 'SQL', 'IT Skills', 'Python', 'Cloud']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Wipro</t>
+          <t>Cyient</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Build the infrastructure required for optimal extraction, transformation, and loading o...</t>
+          <t xml:space="preserve"> Have experience in developing automation frameworksExperience in developing automation ...</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>3-8 Yrs</t>
+          <t>3-6 Yrs</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gurgaon/Gurugram, Bangalore/Bengaluru</t>
+          <t>Bangalore/Bengaluru</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -653,19 +653,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['Snowflake', 'AWS', 'EC2', 'RDS', 'SQL', 'IT Skills', 'Python', 'Cloud']</t>
+          <t>['communication', 'troubleshooting', 'SVN', 'Git', 'automation frameworks', 'Bugzilla', 'Python', 'C programming']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cyient</t>
+          <t>HyrEzy Talent Solutions</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Have experience in developing automation frameworksExperience in developing automation ...</t>
+          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fieldsExp ...</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Bangalore/Bengaluru</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['communication', 'troubleshooting', 'SVN', 'Git', 'automation frameworks', 'Bugzilla', 'Python', 'C programming']</t>
+          <t>['SNS', 'ETL', 'EC2', 'AWS', 'JavaScript', 'Apache', 'REST services', 'Django']</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fieldsExp ...</t>
+          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fields Exp...</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['SNS', 'ETL', 'EC2', 'AWS', 'JavaScript', 'Apache', 'REST services', 'Django']</t>
+          <t>['IT Skills', 'Java', 'Python', 'Javascript', 'AWS', 'S3', 'REST services', 'SQS']</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fields Exp...</t>
+          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fieldsExp ...</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -749,29 +749,29 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['IT Skills', 'Java', 'Python', 'Javascript', 'AWS', 'S3', 'REST services', 'SQS']</t>
+          <t>['SNS', 'ETL', 'EC2', 'AWS', 'JavaScript', 'Apache', 'REST services', 'Django']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>HyrEzy Talent Solutions</t>
+          <t>Verisk Analytics India Private Limited</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Graduate / Post-Graduate in Computer Science / Mathematics/Physics or allied fieldsExp ...</t>
+          <t xml:space="preserve"> Minimum of bachelors degree 4 years development experienceAWS Experience is added advan...</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3-6 Yrs</t>
+          <t>2-4 Yrs</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Hyderabad/Secunderabad</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -781,29 +781,29 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['SNS', 'ETL', 'EC2', 'AWS', 'JavaScript', 'Apache', 'REST services', 'Django']</t>
+          <t>['written communication', 'AJAX', 'JavaScript', 'XML', 'SQL', 'Python', 'AWS', 'IT Skills']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Verisk Analytics India Private Limited</t>
+          <t>Informatica</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Minimum of bachelors degree 4 years development experienceAWS Experience is added advan...</t>
+          <t xml:space="preserve"> In this role, you must be able to work and adapt in a fluid, fast-paced environmentyou ...</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2-4 Yrs</t>
+          <t>4-7 Yrs</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Hyderabad/Secunderabad</t>
+          <t>Bangalore/Bengaluru</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -813,24 +813,24 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['written communication', 'AJAX', 'JavaScript', 'XML', 'SQL', 'Python', 'AWS', 'IT Skills']</t>
+          <t>['Statistical programming', 'Networking', 'Data management', 'Access management', 'devops', 'Informatica', 'SDK', 'Vulnerability management']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Informatica</t>
+          <t xml:space="preserve">ANVETA CONSULTING PRIVATE LIMITED </t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> In this role, you must be able to work and adapt in a fluid, fast-paced environmentyou ...</t>
+          <t xml:space="preserve"> Bachelors Degree in Computer Science or similar fieldAngular is preferred Docker / Cont...</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4-7 Yrs</t>
+          <t>5-10 Yrs</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -845,24 +845,24 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['Statistical programming', 'Networking', 'Data management', 'Access management', 'devops', 'Informatica', 'SDK', 'Vulnerability management']</t>
+          <t>['Fullstack Developer', 'Django', 'React']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve">ANVETA CONSULTING PRIVATE LIMITED </t>
+          <t>Societe Generale Global Solution Centre Pvt Ltd</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Bachelors Degree in Computer Science or similar fieldAngular is preferred Docker / Cont...</t>
+          <t xml:space="preserve"> Create and maintain a operational run book for the teamMonitor the infra capacity and m...</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5-10 Yrs</t>
+          <t>6-7 Yrs</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -877,24 +877,24 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['Fullstack Developer', 'Django', 'React']</t>
+          <t>['IT Skills', 'Python', 'Cloud', 'DevOps', 'Jenkins', 'AWS', 'Azure', 'Application Management']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Societe Generale Global Solution Centre Pvt Ltd</t>
+          <t>Onward Technologies Limited</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Create and maintain a operational run book for the teamMonitor the infra capacity and m...</t>
+          <t xml:space="preserve"> Required key skills are mentioned below, Python &amp; Flask FrameworkWeb application develo...</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6-7 Yrs</t>
+          <t>6-9 Yrs</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -904,66 +904,66 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>10,00,000 - 16,00,000 PA.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>['IT Skills', 'Python', 'Cloud', 'DevOps', 'Jenkins', 'AWS', 'Azure', 'Application Management']</t>
+          <t>['GitHub', 'SQL Server', 'CSS', 'Angular', 'Flask Framework', 'Agile methodology', 'PostgreSQL', 'Microservices']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Onward Technologies Limited</t>
+          <t>Future Focus Infotech Pvt. Ltd.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Required key skills are mentioned below, Python &amp; Flask FrameworkWeb application develo...</t>
+          <t xml:space="preserve"> JOB DESCRIPTION :- Python DeveloperDjango PythonHTMLCSS ExcelHtml5</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6-9 Yrs</t>
+          <t>3-6 Yrs</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bangalore/Bengaluru</t>
+          <t>Kolkata, Hyderabad/Secunderabad, Pune, Ahmedabad, Chennai, Bangalore/Bengaluru, Delhi / NCR, Mumbai (All Areas)</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>10,00,000 - 16,00,000 PA.</t>
+          <t>Not disclosed</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['GitHub', 'SQL Server', 'CSS', 'Angular', 'Flask Framework', 'Agile methodology', 'PostgreSQL', 'Microservices']</t>
+          <t>['CSS', 'HTML', 'Excel', 'Django', 'Html5', 'Python', 'IT Skills', 'Java']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Future Focus Infotech Pvt. Ltd.</t>
+          <t>Societe Generale Global Solution Centre Pvt Ltd</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> JOB DESCRIPTION :- Python DeveloperDjango PythonHTMLCSS ExcelHtml5</t>
+          <t xml:space="preserve"> We are looking for a React.JS developer with working experience on Python Development t...</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>3-6 Yrs</t>
+          <t>4-9 Yrs</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Kolkata, Hyderabad/Secunderabad, Pune, Ahmedabad, Chennai, Bangalore/Bengaluru, Delhi / NCR, Mumbai (All Areas)</t>
+          <t>Bangalore/Bengaluru</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -973,24 +973,24 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['CSS', 'HTML', 'Excel', 'Django', 'Html5', 'Python', 'IT Skills', 'Java']</t>
+          <t>['Front End', 'Html5', 'JavaScript', 'PHP', 'HTML', 'React.js', 'Angular', 'Python']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Societe Generale Global Solution Centre Pvt Ltd</t>
+          <t>Catalyst</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> We are looking for a React.JS developer with working experience on Python Development t...</t>
+          <t xml:space="preserve"> Build and maintain real-time / batch data pipelines that can consolidate and clean up u...</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4-9 Yrs</t>
+          <t>3-8 Yrs</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['Front End', 'Html5', 'JavaScript', 'PHP', 'HTML', 'React.js', 'Angular', 'Python']</t>
+          <t>['IT Skills', 'Java', 'Python', 'Data Science', 'Machine Learning', 'Big Data', 'Hive', 'Data Pipeline']</t>
         </is>
       </c>
     </row>

</xml_diff>